<commit_message>
Formal Design Proposal Updated
Formal Design Proposal has been updated. Letter of Transmittal written
and ready for review. Risk Assessment and Contingency Planning
statements filled in. Dates of decisions to be determined.
</commit_message>
<xml_diff>
--- a/Robot/Formal Design Proposal - Risk Assessment and Contingency Planning.xlsx
+++ b/Robot/Formal Design Proposal - Risk Assessment and Contingency Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\enph253-2015-team13\Robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>Risk Condition</t>
   </si>
@@ -59,12 +59,6 @@
     <t>Arm Risks</t>
   </si>
   <si>
-    <t>Arm cannot locate pets (after pet tape marking is found)</t>
-  </si>
-  <si>
-    <t>Arm is unable to release pets onto basket</t>
-  </si>
-  <si>
     <t>Arm is unable to locate basket, leading to misplaced release of pets</t>
   </si>
   <si>
@@ -74,24 +68,15 @@
     <t>Basket Risks</t>
   </si>
   <si>
+    <t>Basket catapult is unable to launch three pets into the rescue area</t>
+  </si>
+  <si>
     <t>Basket is unable to locate and grab the zipline</t>
   </si>
   <si>
-    <t>Basket is unable to detach from the robot once attached to the zipline</t>
-  </si>
-  <si>
     <t>Driver System Risks</t>
   </si>
   <si>
-    <t>Driver System's optimal speed is too slow to be considered a competitive speed</t>
-  </si>
-  <si>
-    <t>Driver System is unable to carry robot over the ramp</t>
-  </si>
-  <si>
-    <t>Driver System's optimal speed is too fast for the tape follower to keep up</t>
-  </si>
-  <si>
     <t>Tape Follower loses sight of the tape, especially when making turns at corners</t>
   </si>
   <si>
@@ -107,17 +92,167 @@
     <t>Construction Risks</t>
   </si>
   <si>
-    <t>Basket catapult launches the  three pets short of the rescue area</t>
-  </si>
-  <si>
-    <t>Basket catapult launches the three pets too early (i.e. Down the ramp)</t>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Chassis redesign to allow easier access to components, such as a chassis that incoroporates a large opening. Smaller components such as PCB's can also be mounted outside of the chassis rather than inside.</t>
+  </si>
+  <si>
+    <t>Chassis redesign to allow more space claim for more components. Smaller components such as PCB's can also be mounted outside of the chassis rather than inside.</t>
+  </si>
+  <si>
+    <t>Arm cannot locate first pets (after pet tape marking is found)</t>
+  </si>
+  <si>
+    <t>Arm cannot locate pets (either due to the arm being too long or short)</t>
+  </si>
+  <si>
+    <t>Recalibrate the potentiometer/s used on the robotic arm so that it utilizes the correct angles that allows for effective pet release.</t>
+  </si>
+  <si>
+    <t>Recalibrate the potentiometer/s used on the robotic arm so that it utilizes the correct angles that allows for effective pet retrieval.</t>
+  </si>
+  <si>
+    <t>Redsign the arm with different dimensions in order to reach a wider area. Another option is to change the placement of the arm on the chassis.</t>
+  </si>
+  <si>
+    <t>Arm is unable to release pets onto basket using an electromagnet</t>
+  </si>
+  <si>
+    <t>Pet release mechanism will be switched with an aluminum plate that separates a magnet on the arm with the magnet on the pet. A motor will turn the plate to separate the two magnets once the pet is on top of the basket.</t>
+  </si>
+  <si>
+    <t>Pet retrieval becomes a major issue, preventing our robot from scoring points. Recalbiration of the arm's potentionmeters would be required.</t>
+  </si>
+  <si>
+    <t>Pet retrieval becomes a major issue, preventing our robot from scoring points. A redesign to the arm and/or its placement must be conducted.</t>
+  </si>
+  <si>
+    <t>Pet retrieval becomes a major issue, preventing our robot from scoring points. Design would require an aluminum plate and another motor.</t>
+  </si>
+  <si>
+    <t>It will be difficult to conduct maintenance, testing, and replacement tasks on the robot's components.</t>
+  </si>
+  <si>
+    <t>Components such as the robotic arm and circuits will not be included in the robot. Redesign of components or chassis may be required.</t>
+  </si>
+  <si>
+    <t>Recalibration of the tape following system will most likely be conducted. Another option would be to change the placement of the arm so that it does not significantly distort the performance of the tape follower, but is not recommended.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tape following system becomes flawed due to extra mass on top of the sensors (pivot of the robot). </t>
+  </si>
+  <si>
+    <t>Affects strategy of guaranteeing at least three points when scoring. This will either require different torsion springs must be used, or a redesign of the release mechanism depending on the situation.</t>
+  </si>
+  <si>
+    <t>If the issue is a result of the torsion springs not being strong enough to catapult the pets into rescue area, then the torsion springs need only be replaced by stronger ones (a redesign of the basket may be required to accommodate larger springs). The more likely scenario would be that the release mechanism does not activate properly, which would require a redesign of the whole mechanism.</t>
+  </si>
+  <si>
+    <t>Rather than an accordion linkage, the basket would utilize a pulley system to rise up in order to grab the zipline.</t>
+  </si>
+  <si>
+    <t>Accordion linkage does not allow the basket to rise up in order to grab the zipline, or the motor is too weak to lengthen the linkage. All of these issues would likely be due to friction.  Grabbing the zipline, however, would require a redesign of the grabbing mechanism. Overall, this prevents the robot from delivering the last three pets, which is a majority of the points.</t>
+  </si>
+  <si>
+    <t>It affects the delivery of the last three pets if the basket gets stuck on the surface attached to the linkage.</t>
+  </si>
+  <si>
+    <t>A redesign of the accordion linkage's surface where the basket will sit on will be required to minimize the chances of the basket getting stuck.</t>
+  </si>
+  <si>
+    <t>Basket is unable to separate from the robot once attached to the zipline</t>
+  </si>
+  <si>
+    <t>The drive system would need to be recalibrated, which would require additional time.</t>
+  </si>
+  <si>
+    <t>Different sizes of drive gears and or wheels may need to be fabricated in order to change the power output of the motors. Other options include changing the power input into the motor, or using different motors for the drive system altogether.</t>
+  </si>
+  <si>
+    <t>Driver System's optimal speed is too slow to be considered a competitive speed and/or carry the robot over the ramp</t>
+  </si>
+  <si>
+    <t>Gear ratio required for the design is unrealistic in terms of creating the gear</t>
+  </si>
+  <si>
+    <t>Gear ratio determined must be altered to accommodate a more realistic gear ratio.</t>
+  </si>
+  <si>
+    <t>If the gear required for the design is unrealistic in terms of size and number of teeth, then the components that use these gears must be altered in order to accommodate more realistic gears. If the material used for the gears is too weak to handle the torque placed upon it, then the material needs to be stronger. Otherwise, different dimensions for the gear must be used.</t>
+  </si>
+  <si>
+    <t>Affects the overall strategy for the competition if the robot is unable to effectively follow the tape. Many calibration tests would be required.</t>
+  </si>
+  <si>
+    <t>Many calibration tests must be conducted on the robot with most, if not all, of its components installed. This would be time consuming but essential, so the assigned team member who will be conducting these tests will be occupied for the duration of the tests.</t>
+  </si>
+  <si>
+    <t>The robot would be unable to detect the IR beam, which locates the final pet, as well as the zipline.</t>
+  </si>
+  <si>
+    <t>The IR detection circuit must be redesigned in order to accommodate a wider range.</t>
+  </si>
+  <si>
+    <t>An issue of communication between the TINAH and the component will affect the overall strategy for the competition.</t>
+  </si>
+  <si>
+    <t>Electrical circuits for communication between the TINAH and the component must be redesigned more increased reliability.</t>
+  </si>
+  <si>
+    <t>Project productivity would be temporarily decreased, as there are less members of the team present.</t>
+  </si>
+  <si>
+    <t>All team members must be proficient at all of the tasks given in the task list, and must be ready to fill in for the absent member. The absent member may also provide guidelines to their current task for their temporary replacement prior to their absence.</t>
+  </si>
+  <si>
+    <t>A team member becomes temporarily or permanently unavailable to work on the project</t>
+  </si>
+  <si>
+    <t>Accordion linkage is not built reasonably straight, and may have additional friction due to dissimilar lengths of links</t>
+  </si>
+  <si>
+    <t>Refabrication of links would be required in order to fabricate a more effective accordion linkage.</t>
+  </si>
+  <si>
+    <t>Accordion links must  have the same lengths and rivoted in the exact same places. The accuracy of this process is crucial for the effectiveness of the linkage, seeing as that it determines the delivery of the last three pets.</t>
+  </si>
+  <si>
+    <t>Size of gears are unrealistic in terms of the amount of space claim available for the gears.</t>
+  </si>
+  <si>
+    <t>Depending on the gear calculations, some gears may be too big to realistically or effectively fit in the robot.</t>
+  </si>
+  <si>
+    <t>Recalculation of the gear calculations must be conducted, taking into account any newly found constratints of the robot's space claim.</t>
+  </si>
+  <si>
+    <t>A team member is found to have a bigger workload than he can handle</t>
+  </si>
+  <si>
+    <t>Individual productivity would decrease donsidering the amount of workload the team member has.</t>
+  </si>
+  <si>
+    <t>Some of the team member's workload will be distributed evenly to all team members, or covered by another team member with a relatively smaller workload.</t>
+  </si>
+  <si>
+    <t>A team member is found to have a small amount of tasks to conduct at a given time</t>
+  </si>
+  <si>
+    <t>Individual productivity would not be used to its maximum potential</t>
+  </si>
+  <si>
+    <t>The team member will be assigned additional tasks, either help another team member with their task at the discretion of both team members, and enhancing tasks such as planning redesigns, component testing, etc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +260,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +293,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -229,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -243,19 +403,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -281,6 +432,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,16 +731,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -594,265 +765,384 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="B12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="B19" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B20" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B21" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
+    <row r="25" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+    <row r="29" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A26:E26"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
     <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>